<commit_message>
feat(dashboard): remove low stock products card and replace with daily operations table feat(productos): add buttons for downloading and importing adjustment templates; implement Excel import functionality feat(productos): add functionality to process adjustment data from Excel feat(reportes): update button labels for clarity and add export functionality fix(ventas): adjust search input styling for better responsiveness fix(app.menu): update report label for consistency feat(operaciones): create service for managing operations data feat(tabla-operaciones): implement operations table with filtering and data fetching
</commit_message>
<xml_diff>
--- a/src/assets/plantillas/Plantilla_Cargue_Productos.xlsx
+++ b/src/assets/plantillas/Plantilla_Cargue_Productos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduar\OneDrive\Documentos\REPOSITORIOS APP\appoasis\src\assets\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAA141D-235B-4BDD-8C2C-8DFA9D58D1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067493B2-28FB-4746-9B56-5A2A1C349A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{F08F5BB6-B737-4B5E-BA63-C9E5273C1DEA}"/>
   </bookViews>
@@ -34,12 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Nombre</t>
-  </si>
-  <si>
-    <t>Código Barras</t>
   </si>
   <si>
     <t>N° Lote</t>
@@ -416,44 +413,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6FF5A87-564C-4423-A88F-89F6581D520D}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: actualizar títulos de módulos y mejorar visualización de productos
</commit_message>
<xml_diff>
--- a/src/assets/plantillas/Plantilla_Cargue_Productos.xlsx
+++ b/src/assets/plantillas/Plantilla_Cargue_Productos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduar\OneDrive\Documentos\REPOSITORIOS APP\appoasis\src\assets\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067493B2-28FB-4746-9B56-5A2A1C349A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3A1D2A-FAE2-4C6D-BA98-809F5B29AC6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{F08F5BB6-B737-4B5E-BA63-C9E5273C1DEA}"/>
   </bookViews>
@@ -34,17 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Nombre</t>
   </si>
   <si>
-    <t>N° Lote</t>
-  </si>
-  <si>
-    <t>Fecha Vencimiento</t>
-  </si>
-  <si>
     <t>Laboratorio</t>
   </si>
   <si>
@@ -55,6 +49,9 @@
   </si>
   <si>
     <t>Presentación</t>
+  </si>
+  <si>
+    <t>Precio Costo</t>
   </si>
 </sst>
 </file>
@@ -413,40 +410,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6FF5A87-564C-4423-A88F-89F6581D520D}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>